<commit_message>
Add passive event check-ins and Mixtacular pull hat. Resolves #51.
</commit_message>
<xml_diff>
--- a/doc/hats_and_camos.xlsx
+++ b/doc/hats_and_camos.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\workspace_v6_1_3\qc13\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glouthan\workspace_v6_1_3\qc13\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Camos" sheetId="2" r:id="rId2"/>
     <sheet name="Event check-ins" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="279">
   <si>
     <t>Achievement</t>
   </si>
@@ -857,12 +857,18 @@
   </si>
   <si>
     <t>Weatherqueer</t>
+  </si>
+  <si>
+    <t>Impl?</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1264,1332 +1270,1389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D2:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>136</v>
       </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G33" si="0">CONCATENATE("#define ", E2, " ", A2)</f>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="0">CONCATENATE("#define ", F2, " ", B2)</f>
         <v>#define HAT_GEORGE 0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>136</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_EVAN 1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>136</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_TPROPHET 2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>136</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_ZAC 3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>136</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_ERIC 4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>136</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_SHAUN 5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>136</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_MARCUS 6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B9">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>136</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_JASON 7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>136</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_AARON 8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>136</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_JONATHAN 9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>278</v>
+      </c>
+      <c r="B12">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>136</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_JAKE 10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>136</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_COLLIN 11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>136</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_ALYSSA 12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B15">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>137</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_DONOR_REED 13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>137</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_DONOR_HEATHER 14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>278</v>
+      </c>
+      <c r="B17">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>3</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>137</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_DONOR_ERIC 15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>278</v>
+      </c>
+      <c r="B18">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>137</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_DONOR_CHRIS 16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>170</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>138</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_BADGE_TALK 17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>3</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>139</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_POOL_FIRST 18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>3</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>140</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_POOL_LAST 19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>3</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>141</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_MIXER_SAT_FIRST 20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>171</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>142</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_KARAOKE_FIRST 21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>3</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>172</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>143</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_KARAOKE_LAST 22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>173</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>144</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_PEST 23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>145</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_MORNING 24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>5</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>175</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>146</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_HOT_COLD 25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>5</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>176</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>147</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_BRIGHT_DARK 26</v>
       </c>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>5</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>177</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>148</v>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_COLD 27</v>
       </c>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>5</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>178</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>149</v>
       </c>
-      <c r="G30" t="str">
+      <c r="H30" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_HOT 28</v>
       </c>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>5</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>179</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>150</v>
       </c>
-      <c r="G31" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_MATE_UBER 29</v>
       </c>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32">
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>5</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>180</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>151</v>
       </c>
-      <c r="G32" t="str">
+      <c r="H32" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_MATE_HANDLER 30</v>
       </c>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33">
         <v>31</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>5</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>181</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>152</v>
       </c>
-      <c r="G33" t="str">
+      <c r="H33" t="str">
         <f t="shared" si="0"/>
         <v>#define HAT_MATE_50 31</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34">
         <v>32</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>5</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>182</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>153</v>
       </c>
-      <c r="G34" t="str">
-        <f t="shared" ref="G34:G58" si="1">CONCATENATE("#define ", E34, " ", A34)</f>
+      <c r="H34" t="str">
+        <f t="shared" ref="H34:H58" si="1">CONCATENATE("#define ", F34, " ", B34)</f>
         <v>#define HAT_MATE_100 32</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35">
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>5</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>183</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>154</v>
       </c>
-      <c r="G35" t="str">
+      <c r="H35" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_MATE_200 33</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36">
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>5</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>184</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>155</v>
       </c>
-      <c r="G36" t="str">
+      <c r="H36" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_DINK_50 34</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>35</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>5</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>156</v>
       </c>
-      <c r="G37" t="str">
+      <c r="H37" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_TIME_NEAR_UBERS 35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>36</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>5</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>157</v>
       </c>
-      <c r="G38" t="str">
+      <c r="H38" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_NEAR_HANDLERS 36</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39">
         <v>37</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>5</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>158</v>
       </c>
-      <c r="G39" t="str">
+      <c r="H39" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_TIME_NEAR_HANDLERS 37</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>278</v>
+      </c>
+      <c r="B40">
         <v>38</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>5</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>185</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>159</v>
       </c>
-      <c r="G40" t="str">
+      <c r="H40" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_ALL_MIXERS 38</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41">
         <v>39</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>160</v>
       </c>
-      <c r="G41" t="str">
+      <c r="H41" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_KONAMI 39</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42">
         <v>40</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>5</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>186</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>161</v>
       </c>
-      <c r="G42" t="str">
+      <c r="H42" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_MINUTEMAN 40</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>41</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>5</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>162</v>
       </c>
-      <c r="G43" t="str">
+      <c r="H43" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_POWER_CYCLES 41</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44">
         <v>42</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>5</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>163</v>
       </c>
-      <c r="G44" t="str">
+      <c r="H44" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_SUPER_INK 42</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45">
         <v>43</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>5</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>164</v>
       </c>
-      <c r="G45" t="str">
+      <c r="H45" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_MARGIN_HIGH 43</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46">
         <v>44</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>5</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>165</v>
       </c>
-      <c r="G46" t="str">
+      <c r="H46" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_MARGIN_LOW 44</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47">
         <v>45</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>5</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>166</v>
       </c>
-      <c r="G47" t="str">
+      <c r="H47" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_LOW_MARGIN 45</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48">
         <v>46</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>5</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>47</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>167</v>
       </c>
-      <c r="G48" t="str">
+      <c r="H48" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_BORROWER 46</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49">
         <v>47</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G49" t="str">
+      <c r="H49" t="str">
         <f t="shared" si="1"/>
         <v>#define  47</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50">
         <v>48</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G50" t="str">
+      <c r="H50" t="str">
         <f t="shared" si="1"/>
         <v>#define  48</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51">
         <v>49</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G51" t="str">
+      <c r="H51" t="str">
         <f t="shared" si="1"/>
         <v>#define  49</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>48</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>5</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>187</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>168</v>
       </c>
-      <c r="G52" t="str">
+      <c r="H52" t="str">
         <f t="shared" si="1"/>
         <v>#define  50</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>135</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>133</v>
       </c>
-      <c r="G53" t="str">
+      <c r="H53" t="str">
         <f t="shared" si="1"/>
         <v>#define  51</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>135</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>133</v>
       </c>
-      <c r="G54" t="str">
+      <c r="H54" t="str">
         <f t="shared" si="1"/>
         <v>#define  52</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>135</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>133</v>
       </c>
-      <c r="G55" t="str">
+      <c r="H55" t="str">
         <f t="shared" si="1"/>
         <v>#define  53</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>135</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>133</v>
       </c>
-      <c r="G56" t="str">
+      <c r="H56" t="str">
         <f t="shared" si="1"/>
         <v>#define  54</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>81</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>83</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="F57" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>169</v>
       </c>
-      <c r="G57" t="str">
+      <c r="H57" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_UBER 55</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>82</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>83</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="F58" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>102</v>
       </c>
-      <c r="G58" t="str">
+      <c r="H58" t="str">
         <f t="shared" si="1"/>
         <v>#define HAT_HANDLER 56</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C49 C52:C1048576">
+  <conditionalFormatting sqref="D1:D49 D52:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"PULL"</formula>
     </cfRule>
@@ -2610,7 +2673,7 @@
   <dimension ref="B1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,7 +2729,7 @@
       <c r="B5" t="s">
         <v>193</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>221</v>
       </c>
       <c r="D5" t="s">
@@ -2688,7 +2751,7 @@
       <c r="B7" t="s">
         <v>195</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>229</v>
       </c>
       <c r="D7" t="s">
@@ -2754,7 +2817,7 @@
       <c r="B13" t="s">
         <v>201</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>225</v>
       </c>
       <c r="D13" t="s">
@@ -2776,7 +2839,7 @@
       <c r="B15" t="s">
         <v>204</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D15" t="s">
@@ -2787,7 +2850,7 @@
       <c r="B16" t="s">
         <v>203</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>228</v>
       </c>
       <c r="D16" t="s">
@@ -2798,7 +2861,7 @@
       <c r="B17" t="s">
         <v>205</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>231</v>
       </c>
       <c r="D17" t="s">
@@ -2853,7 +2916,7 @@
       <c r="B22" t="s">
         <v>210</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>216</v>
       </c>
       <c r="D22" t="s">
@@ -2864,7 +2927,7 @@
       <c r="B23" t="s">
         <v>211</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>217</v>
       </c>
       <c r="D23" t="s">
@@ -2875,7 +2938,7 @@
       <c r="B24" t="s">
         <v>212</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>218</v>
       </c>
       <c r="D24" t="s">
@@ -2886,7 +2949,7 @@
       <c r="B25" t="s">
         <v>213</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>219</v>
       </c>
       <c r="D25" t="s">
@@ -2948,7 +3011,7 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Re-do konami code, resolving #61.
</commit_message>
<xml_diff>
--- a/doc/hats_and_camos.xlsx
+++ b/doc/hats_and_camos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hats" sheetId="1" r:id="rId1"/>
@@ -766,9 +766,6 @@
     <t>Attend Women of QC.</t>
   </si>
   <si>
-    <t>^ ^ v v &lt; &gt; &lt; &gt; A B START.</t>
-  </si>
-  <si>
     <t>Attend QC trans meetup.</t>
   </si>
   <si>
@@ -863,6 +860,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>^ ^ v v &lt; &gt; &lt; &gt; B A START.</t>
   </si>
 </sst>
 </file>
@@ -1272,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1288,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B15">
         <v>13</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -1961,7 +1961,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1985,7 +1985,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B40">
         <v>38</v>
@@ -2672,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2708,10 +2708,10 @@
         <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -2733,7 +2733,7 @@
         <v>221</v>
       </c>
       <c r="D5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2744,7 +2744,7 @@
         <v>222</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2777,7 +2777,7 @@
         <v>224</v>
       </c>
       <c r="D9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
         <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -2799,7 +2799,7 @@
         <v>230</v>
       </c>
       <c r="D11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -2810,7 +2810,7 @@
         <v>215</v>
       </c>
       <c r="D12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -2821,7 +2821,7 @@
         <v>225</v>
       </c>
       <c r="D13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -2832,7 +2832,7 @@
         <v>226</v>
       </c>
       <c r="D14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -2843,7 +2843,7 @@
         <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -2854,7 +2854,7 @@
         <v>228</v>
       </c>
       <c r="D16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -2865,7 +2865,7 @@
         <v>231</v>
       </c>
       <c r="D17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -2876,7 +2876,7 @@
         <v>232</v>
       </c>
       <c r="D18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -2884,10 +2884,10 @@
         <v>207</v>
       </c>
       <c r="C19" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" t="s">
         <v>251</v>
-      </c>
-      <c r="D19" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -2920,7 +2920,7 @@
         <v>216</v>
       </c>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -2931,7 +2931,7 @@
         <v>217</v>
       </c>
       <c r="D23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -2942,7 +2942,7 @@
         <v>218</v>
       </c>
       <c r="D24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -2953,7 +2953,7 @@
         <v>219</v>
       </c>
       <c r="D25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -2964,7 +2964,7 @@
         <v>239</v>
       </c>
       <c r="D26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -2975,7 +2975,7 @@
         <v>240</v>
       </c>
       <c r="D27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
         <v>241</v>
       </c>
       <c r="D28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -2997,7 +2997,7 @@
         <v>242</v>
       </c>
       <c r="D29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3056,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some hats. Resolve #58.
</commit_message>
<xml_diff>
--- a/doc/hats_and_camos.xlsx
+++ b/doc/hats_and_camos.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="280">
   <si>
     <t>Achievement</t>
   </si>
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,6 +1768,9 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>277</v>
+      </c>
       <c r="B19">
         <v>17</v>
       </c>
@@ -1792,6 +1795,9 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>277</v>
+      </c>
       <c r="B20">
         <v>18</v>
       </c>
@@ -1816,6 +1822,9 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>277</v>
+      </c>
       <c r="B21">
         <v>19</v>
       </c>
@@ -1840,6 +1849,9 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>277</v>
+      </c>
       <c r="B22">
         <v>20</v>
       </c>
@@ -1864,6 +1876,9 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>277</v>
+      </c>
       <c r="B23">
         <v>21</v>
       </c>
@@ -1888,6 +1903,9 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>277</v>
+      </c>
       <c r="B24">
         <v>22</v>
       </c>
@@ -2181,6 +2199,9 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>277</v>
+      </c>
       <c r="B36">
         <v>34</v>
       </c>
@@ -2352,6 +2373,9 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>277</v>
+      </c>
       <c r="B43">
         <v>41</v>
       </c>
@@ -2376,6 +2400,9 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>277</v>
+      </c>
       <c r="B44">
         <v>42</v>
       </c>
@@ -2472,6 +2499,9 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>277</v>
+      </c>
       <c r="B48">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Add tons of hats and camos. Getting there!!!!!
</commit_message>
<xml_diff>
--- a/doc/hats_and_camos.xlsx
+++ b/doc/hats_and_camos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hats" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="280">
   <si>
     <t>Achievement</t>
   </si>
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,6 +2205,9 @@
       <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>270</v>
+      </c>
       <c r="B31">
         <v>29</v>
       </c>
@@ -2234,6 +2237,9 @@
       <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>270</v>
+      </c>
       <c r="B32">
         <v>30</v>
       </c>
@@ -2263,6 +2269,9 @@
       <c r="K32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>270</v>
+      </c>
       <c r="B33">
         <v>31</v>
       </c>
@@ -2291,6 +2300,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>270</v>
+      </c>
       <c r="B34">
         <v>32</v>
       </c>
@@ -2319,6 +2331,9 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>270</v>
+      </c>
       <c r="B35">
         <v>33</v>
       </c>
@@ -2422,15 +2437,15 @@
         <v>117</v>
       </c>
       <c r="G38" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="2"/>
         <v>#define HAT_NEAR_HANDLERS 36</v>
       </c>
-      <c r="I38" t="str">
-        <f t="shared" si="1"/>
-        <v>36: ("Handler-on", "Spend hours near a handler."),</v>
+      <c r="I38" t="e">
+        <f>_xlfn.CONCAT(B38,": (""", C38, """, ", """",#REF!, """),")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2450,14 +2465,14 @@
         <v>116</v>
       </c>
       <c r="G39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="2"/>
         <v>#define HAT_TIME_NEAR_HANDLERS 37</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B39,": (""", C39, """, ", """", G38, """),")</f>
         <v>37: ("Controlled crowd", "Be near all on-duty handlers."),</v>
       </c>
     </row>
@@ -2728,7 +2743,7 @@
         <v>46: ("Imposter", "Borrow a hat. Or cheat."),</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>47</v>
       </c>
@@ -2744,7 +2759,7 @@
         <v>47: ("blue spare", ""),</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>48</v>
       </c>
@@ -2760,7 +2775,7 @@
         <v>48: ("blue spare", ""),</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>49</v>
       </c>
@@ -2776,11 +2791,14 @@
         <v>49: ("blue spare", ""),</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>270</v>
+      </c>
       <c r="B52">
         <v>50</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D52" t="s">
@@ -2804,7 +2822,7 @@
         <v>50: ("Contest", "Figure it out."),</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>51</v>
       </c>
@@ -2823,7 +2841,7 @@
         <v>51: ("black spare", ""),</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>52</v>
       </c>
@@ -2842,7 +2860,7 @@
         <v>52: ("black spare", ""),</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>53</v>
       </c>
@@ -2861,7 +2879,7 @@
         <v>53: ("black spare", ""),</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>54</v>
       </c>
@@ -2880,7 +2898,7 @@
         <v>54: ("black spare", ""),</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>55</v>
       </c>
@@ -2905,7 +2923,7 @@
         <v>55: ("Uber", "Be uber."),</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>56</v>
       </c>
@@ -2949,10 +2967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2963,7 +2981,7 @@
     <col min="11" max="11" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>182</v>
       </c>
@@ -2971,7 +2989,10 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>270</v>
+      </c>
       <c r="B2" t="s">
         <v>183</v>
       </c>
@@ -2982,7 +3003,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>184</v>
       </c>
@@ -2993,7 +3014,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>185</v>
       </c>
@@ -3004,7 +3025,10 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>270</v>
+      </c>
       <c r="B5" t="s">
         <v>186</v>
       </c>
@@ -3015,7 +3039,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>187</v>
       </c>
@@ -3026,7 +3050,10 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>270</v>
+      </c>
       <c r="B7" t="s">
         <v>188</v>
       </c>
@@ -3037,7 +3064,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>189</v>
       </c>
@@ -3048,7 +3075,10 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>270</v>
+      </c>
       <c r="B9" t="s">
         <v>190</v>
       </c>
@@ -3059,7 +3089,10 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>270</v>
+      </c>
       <c r="B10" t="s">
         <v>191</v>
       </c>
@@ -3070,7 +3103,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>192</v>
       </c>
@@ -3081,7 +3114,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>193</v>
       </c>
@@ -3092,7 +3125,10 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>270</v>
+      </c>
       <c r="B13" t="s">
         <v>194</v>
       </c>
@@ -3103,7 +3139,10 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>270</v>
+      </c>
       <c r="B14" t="s">
         <v>195</v>
       </c>
@@ -3114,7 +3153,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>270</v>
+      </c>
       <c r="B15" t="s">
         <v>197</v>
       </c>
@@ -3125,7 +3167,10 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>270</v>
+      </c>
       <c r="B16" t="s">
         <v>196</v>
       </c>
@@ -3136,7 +3181,10 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>270</v>
+      </c>
       <c r="B17" t="s">
         <v>198</v>
       </c>
@@ -3147,7 +3195,10 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>270</v>
+      </c>
       <c r="B18" t="s">
         <v>199</v>
       </c>
@@ -3158,7 +3209,10 @@
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>270</v>
+      </c>
       <c r="B19" t="s">
         <v>200</v>
       </c>
@@ -3169,7 +3223,10 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>270</v>
+      </c>
       <c r="B20" t="s">
         <v>201</v>
       </c>
@@ -3180,7 +3237,10 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>270</v>
+      </c>
       <c r="B21" t="s">
         <v>202</v>
       </c>
@@ -3191,7 +3251,10 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>270</v>
+      </c>
       <c r="B22" t="s">
         <v>203</v>
       </c>
@@ -3202,7 +3265,10 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>270</v>
+      </c>
       <c r="B23" t="s">
         <v>204</v>
       </c>
@@ -3213,7 +3279,10 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>270</v>
+      </c>
       <c r="B24" t="s">
         <v>205</v>
       </c>
@@ -3224,7 +3293,10 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>270</v>
+      </c>
       <c r="B25" t="s">
         <v>206</v>
       </c>
@@ -3235,7 +3307,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>270</v>
+      </c>
       <c r="B26" t="s">
         <v>228</v>
       </c>
@@ -3246,7 +3321,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>270</v>
+      </c>
       <c r="B27" t="s">
         <v>231</v>
       </c>
@@ -3257,7 +3335,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
       <c r="B28" t="s">
         <v>229</v>
       </c>
@@ -3268,7 +3349,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>270</v>
+      </c>
       <c r="B29" t="s">
         <v>230</v>
       </c>

</xml_diff>

<commit_message>
Konami code and counting!
</commit_message>
<xml_diff>
--- a/doc/hats_and_camos.xlsx
+++ b/doc/hats_and_camos.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glouthan\workspace_v6_1_3\qc13\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\workspace_v6_1_3\qc13\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Hats" sheetId="1" r:id="rId1"/>
     <sheet name="Camos" sheetId="2" r:id="rId2"/>
     <sheet name="Event check-ins" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="280">
   <si>
     <t>Achievement</t>
   </si>
@@ -871,7 +871,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,6 +2022,9 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
       <c r="B25">
         <v>23</v>
       </c>
@@ -2050,6 +2053,9 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
       <c r="B26">
         <v>24</v>
       </c>
@@ -2393,6 +2399,9 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>270</v>
+      </c>
       <c r="B37">
         <v>35</v>
       </c>
@@ -2421,6 +2430,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>270</v>
+      </c>
       <c r="B38">
         <v>36</v>
       </c>
@@ -2449,6 +2461,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>270</v>
+      </c>
       <c r="B39">
         <v>37</v>
       </c>
@@ -2508,6 +2523,9 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>270</v>
+      </c>
       <c r="B41">
         <v>39</v>
       </c>
@@ -2629,6 +2647,9 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>270</v>
+      </c>
       <c r="B45">
         <v>43</v>
       </c>
@@ -2657,6 +2678,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>270</v>
+      </c>
       <c r="B46">
         <v>44</v>
       </c>
@@ -2685,6 +2709,9 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>270</v>
+      </c>
       <c r="B47">
         <v>45</v>
       </c>
@@ -2969,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix hat detection & sweep up TODOs.
</commit_message>
<xml_diff>
--- a/doc/hats_and_camos.xlsx
+++ b/doc/hats_and_camos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Hats" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="280">
   <si>
     <t>Achievement</t>
   </si>
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3143,6 +3143,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>270</v>
+      </c>
       <c r="B11" t="s">
         <v>192</v>
       </c>

</xml_diff>